<commit_message>
Override Feature File implemented with apache poi
</commit_message>
<xml_diff>
--- a/src/test/resources/dataprovider/TestData.xlsx
+++ b/src/test/resources/dataprovider/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sures\Desktop\cucumber\src\test\resources\dataprovider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sures\Desktop\testngwithlatest\src\test\resources\dataprovider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D4699A-187A-4E4B-B622-3D937CBD7D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFD2B26-BC09-4141-A55F-D0B5BDDB0E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Scenario</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>lastRow</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>